<commit_message>
Update Inventory inscribed pieces.xlsx
</commit_message>
<xml_diff>
--- a/metadata/Inventory inscribed pieces.xlsx
+++ b/metadata/Inventory inscribed pieces.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenttournier/Dropbox/Recherche/Projets_Recherche/Kanaganahalli/Kanaghanahalli_Inscriptions/Metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenttournier/Documents/GitHub/tfb-satavahana-epigraphy/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447123F9-74D4-D147-A568-F98971EC46C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB67406-C479-2E4D-8E82-33329CEEBD1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2560" windowWidth="39400" windowHeight="19860" xr2:uid="{D79794C4-FCC0-9B4A-B6F1-FEEF81BE6884}"/>
   </bookViews>
@@ -2766,8 +2766,8 @@
   <dimension ref="A1:M433"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F309" sqref="F309"/>
+      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F217" sqref="F217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>